<commit_message>
refined tests to cover corner case of double project column
</commit_message>
<xml_diff>
--- a/test/assets/2016_timesheet_Luca-Pacioli.xlsx
+++ b/test/assets/2016_timesheet_Luca-Pacioli.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2016-1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="255">
   <si>
     <t>STICHTING DYNE.ORG</t>
   </si>
@@ -555,6 +555,9 @@
     <t>due</t>
   </si>
   <si>
+    <t>alpha</t>
+  </si>
+  <si>
     <t>2016-8-10</t>
   </si>
   <si>
@@ -570,6 +573,12 @@
     <t>2016-9</t>
   </si>
   <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
     <t>Thu 1</t>
   </si>
   <si>
@@ -783,7 +792,7 @@
     <t>quattro</t>
   </si>
   <si>
-    <t>T1.1</t>
+    <t>delta</t>
   </si>
   <si>
     <t>Sat 31</t>
@@ -1022,15 +1031,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>189360</xdr:colOff>
+      <xdr:colOff>216360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>545400</xdr:colOff>
+      <xdr:colOff>572040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1043,8 +1052,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2646720" y="0"/>
-          <a:ext cx="1518120" cy="1019880"/>
+          <a:off x="2931480" y="0"/>
+          <a:ext cx="1643400" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1064,15 +1073,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190800</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>571320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1085,8 +1094,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514600" y="0"/>
-          <a:ext cx="1515960" cy="1019880"/>
+          <a:off x="2793240" y="0"/>
+          <a:ext cx="1641240" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1106,15 +1115,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190800</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>545040</xdr:colOff>
+      <xdr:colOff>571680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1127,8 +1136,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514600" y="0"/>
-          <a:ext cx="1516320" cy="1020240"/>
+          <a:off x="2793240" y="0"/>
+          <a:ext cx="1641600" cy="1019880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1148,15 +1157,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190440</xdr:colOff>
+      <xdr:colOff>217440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544320</xdr:colOff>
+      <xdr:colOff>570960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1169,8 +1178,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514240" y="0"/>
-          <a:ext cx="1515960" cy="1019880"/>
+          <a:off x="2792880" y="0"/>
+          <a:ext cx="1641240" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1190,15 +1199,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190800</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>545040</xdr:colOff>
+      <xdr:colOff>571680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1211,8 +1220,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2676600" y="0"/>
-          <a:ext cx="1516320" cy="1019880"/>
+          <a:off x="2961000" y="0"/>
+          <a:ext cx="1641600" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1232,15 +1241,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>189360</xdr:colOff>
+      <xdr:colOff>216360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>571320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1253,8 +1262,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2646720" y="0"/>
-          <a:ext cx="1517400" cy="1019880"/>
+          <a:off x="2931480" y="0"/>
+          <a:ext cx="1642680" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1274,15 +1283,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190800</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>545040</xdr:colOff>
+      <xdr:colOff>571680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1295,8 +1304,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2638440" y="0"/>
-          <a:ext cx="1516320" cy="1019880"/>
+          <a:off x="2923200" y="0"/>
+          <a:ext cx="1641960" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1316,15 +1325,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>216000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544320</xdr:colOff>
+      <xdr:colOff>570960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1337,8 +1346,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2855880" y="0"/>
-          <a:ext cx="1517400" cy="1019880"/>
+          <a:off x="3164760" y="0"/>
+          <a:ext cx="1642680" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1358,15 +1367,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190800</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544320</xdr:colOff>
+      <xdr:colOff>570960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1379,8 +1388,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514600" y="0"/>
-          <a:ext cx="1515600" cy="1019880"/>
+          <a:off x="2793240" y="0"/>
+          <a:ext cx="1640880" cy="1019520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1400,15 +1409,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>191160</xdr:colOff>
+      <xdr:colOff>218160</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>571320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1421,8 +1430,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514960" y="0"/>
-          <a:ext cx="1515600" cy="1020240"/>
+          <a:off x="2793600" y="0"/>
+          <a:ext cx="1640880" cy="1019880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1442,15 +1451,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>216000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>571320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1463,8 +1472,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2627280" y="0"/>
-          <a:ext cx="1517760" cy="1020240"/>
+          <a:off x="2912760" y="0"/>
+          <a:ext cx="1643040" cy="1019880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1484,15 +1493,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>191160</xdr:colOff>
+      <xdr:colOff>218160</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>571320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1505,8 +1514,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2514960" y="0"/>
-          <a:ext cx="1515600" cy="1020240"/>
+          <a:off x="2793600" y="0"/>
+          <a:ext cx="1640880" cy="1019880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1528,15 +1537,15 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2163,13 +2172,13 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2180,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2203,7 +2212,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -2216,7 +2225,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2227,7 +2236,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2249,7 +2258,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2264,7 +2273,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2279,7 +2288,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>6</v>
@@ -2296,7 +2305,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>6</v>
@@ -2313,7 +2322,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>6</v>
@@ -2330,7 +2339,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>6</v>
@@ -2347,7 +2356,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>6</v>
@@ -2364,7 +2373,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2379,7 +2388,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2394,7 +2403,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2409,7 +2418,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>6</v>
@@ -2426,7 +2435,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>6</v>
@@ -2443,7 +2452,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -2458,7 +2467,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>6</v>
@@ -2475,7 +2484,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -2490,7 +2499,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -2505,7 +2514,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -2520,7 +2529,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -2535,7 +2544,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>6</v>
@@ -2552,7 +2561,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>6</v>
@@ -2569,7 +2578,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>6</v>
@@ -2586,7 +2595,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -2601,7 +2610,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -2616,7 +2625,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>6</v>
@@ -2633,7 +2642,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>6</v>
@@ -2650,7 +2659,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>6</v>
@@ -2667,7 +2676,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>6</v>
@@ -2684,7 +2693,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>6</v>
@@ -2701,7 +2710,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -2716,7 +2725,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2731,7 +2740,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B41" s="6" t="n">
         <v>6</v>
@@ -2786,7 +2795,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2816,13 +2825,13 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2835,7 +2844,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2860,7 +2869,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -2875,7 +2884,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2886,11 +2895,11 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -3442,7 +3451,7 @@
         <v>40</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3472,13 +3481,13 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3491,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3514,7 +3523,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -3523,38 +3532,44 @@
         <v>173</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -3572,7 +3587,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>5</v>
@@ -3591,7 +3606,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="n">
@@ -3608,7 +3623,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -3623,7 +3638,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3638,7 +3653,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -3655,7 +3670,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>4</v>
@@ -3674,7 +3689,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>4</v>
@@ -3693,7 +3708,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>2</v>
@@ -3712,7 +3727,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>2</v>
@@ -3731,7 +3746,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3746,7 +3761,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -3761,7 +3776,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>6</v>
@@ -3778,7 +3793,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="n">
@@ -3797,7 +3812,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>2</v>
@@ -3818,7 +3833,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>2</v>
@@ -3839,7 +3854,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>2</v>
@@ -3860,7 +3875,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -3875,7 +3890,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -3890,7 +3905,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>2</v>
@@ -3909,7 +3924,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>2</v>
@@ -3930,7 +3945,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>2</v>
@@ -3951,7 +3966,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>2</v>
@@ -3972,7 +3987,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>2</v>
@@ -3991,7 +4006,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -4006,7 +4021,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -4021,7 +4036,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>2</v>
@@ -4038,7 +4053,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>2</v>
@@ -4057,7 +4072,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>2</v>
@@ -4076,7 +4091,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B39" s="6" t="n">
         <v>2</v>
@@ -4095,7 +4110,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>2</v>
@@ -4116,7 +4131,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -4169,7 +4184,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4199,15 +4214,15 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I38" activeCellId="0" sqref="I38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4818,15 +4833,15 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5451,15 +5466,15 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6079,15 +6094,15 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6740,13 +6755,13 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7378,13 +7393,13 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7435,7 +7450,9 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -7989,7 +8006,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8020,15 +8037,15 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8041,7 +8058,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8549,7 +8566,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -8564,7 +8581,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -8648,13 +8665,13 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.12755102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8667,7 +8684,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8695,7 +8712,9 @@
       <c r="C7" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -8705,8 +8724,12 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>181</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -8732,7 +8755,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -8747,7 +8770,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -8762,71 +8785,79 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="6" t="n">
+        <v>6</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="4" t="n">
         <f aca="false">SUM(B13:G13)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="n">
+        <v>6</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4" t="n">
         <f aca="false">SUM(B14:G14)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>6</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="6" t="n">
+        <v>6</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="4" t="n">
         <f aca="false">SUM(B15:G15)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>6</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="n">
+        <v>6</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4" t="n">
         <f aca="false">SUM(B16:G16)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>6</v>
@@ -8843,7 +8874,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>6</v>
@@ -8860,7 +8891,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>6</v>
@@ -8877,22 +8908,24 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="n">
+        <v>6</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="4" t="n">
         <f aca="false">SUM(B20:G20)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -8907,7 +8940,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>6</v>
@@ -8924,56 +8957,62 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>6</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="n">
+        <v>7</v>
+      </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="4" t="n">
         <f aca="false">SUM(B23:G23)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>6</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7" t="n">
+        <v>8</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="4" t="n">
         <f aca="false">SUM(B24:G24)</f>
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="6" t="n">
+        <v>4</v>
+      </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="4" t="n">
         <f aca="false">SUM(B25:G25)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -8988,7 +9027,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -9003,7 +9042,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -9018,7 +9057,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="n">
@@ -9035,7 +9074,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="n">
@@ -9052,7 +9091,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="n">
@@ -9069,7 +9108,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="n">
@@ -9086,7 +9125,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="n">
@@ -9103,7 +9142,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -9118,7 +9157,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -9133,7 +9172,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>6</v>
@@ -9150,7 +9189,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>6</v>
@@ -9167,7 +9206,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -9182,7 +9221,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B39" s="6" t="n">
         <v>6</v>
@@ -9199,7 +9238,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>6</v>
@@ -9225,7 +9264,7 @@
       </c>
       <c r="D41" s="4" t="n">
         <f aca="false">SUM(D11:D40)</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E41" s="4" t="n">
         <f aca="false">SUM(E11:E40)</f>
@@ -9241,7 +9280,7 @@
       </c>
       <c r="H41" s="6" t="n">
         <f aca="false">SUM(H11:H40)</f>
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9254,7 +9293,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>